<commit_message>
added rao1 narrow survey
</commit_message>
<xml_diff>
--- a/results/formatted_excel/traditional_genetic_algorithm_comparison_jan30.xlsx
+++ b/results/formatted_excel/traditional_genetic_algorithm_comparison_jan30.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://livekutztown-my.sharepoint.com/personal/adell892_live_kutztown_edu/Documents/Documents/jbm/results/formatted_excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\antho\OneDrive - Kutztown University\Documents\jbm\results\formatted_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{389A01E6-459C-4C69-8E6B-D6AF1E0836FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="7" r:id="rId1"/>
@@ -137,8 +137,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="165" formatCode="0.000%"/>
-    <numFmt numFmtId="170" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.000%"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -189,9 +189,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -807,7 +807,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA227A51-EE9B-47E5-9A96-7187E44FDACD}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P6" sqref="P6"/>
     </sheetView>
   </sheetViews>
@@ -822,8 +822,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>